<commit_message>
fixed up process, gather doesn't work atm, but worksheets updated, not the finished printer but zip code present and so is date worked header
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>Read Me</t>
   </si>
@@ -156,6 +156,12 @@
     <t>#??</t>
   </si>
   <si>
+    <t>[Zip Code]</t>
+  </si>
+  <si>
+    <t>Date(s) Worked: 0/0/2000</t>
+  </si>
+  <si>
     <t>Street Address</t>
   </si>
   <si>
@@ -255,7 +261,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -276,28 +282,28 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -324,22 +330,22 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
@@ -351,28 +357,28 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thick">
         <color indexed="8"/>
@@ -411,7 +417,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
@@ -446,7 +452,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -455,13 +461,13 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -478,82 +484,82 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="8" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="8" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -562,7 +568,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -574,7 +580,7 @@
     <xf numFmtId="49" fontId="9" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -583,28 +589,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="13" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -624,8 +630,8 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff111111"/>
       <rgbColor rgb="ffb7b7b7"/>
     </indexedColors>
@@ -826,12 +832,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -864,10 +870,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1115,12 +1121,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1435,10 +1441,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2155,12 +2161,16 @@
       <c r="A1" t="s" s="33">
         <v>46</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" t="s" s="34">
+        <v>47</v>
+      </c>
       <c r="C1" s="35"/>
       <c r="D1" s="36"/>
       <c r="E1" s="36"/>
       <c r="F1" s="36"/>
-      <c r="G1" s="37"/>
+      <c r="G1" t="s" s="37">
+        <v>48</v>
+      </c>
       <c r="H1" s="38"/>
       <c r="I1" s="38"/>
       <c r="J1" s="38"/>
@@ -2186,10 +2196,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s" s="39">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s" s="40">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s" s="39">
         <v>14</v>

</xml_diff>